<commit_message>
Minor bugfixes; begin working on orientation calculations
</commit_message>
<xml_diff>
--- a/Host/CommunicationProtocol.xlsx
+++ b/Host/CommunicationProtocol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AppleMath\Documents\APSC200_2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AppleMath\Documents\APSC200_2019\SWEP-2019\Host\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="146">
   <si>
     <t>b15</t>
   </si>
@@ -792,7 +792,7 @@
   <dimension ref="A1:X63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S28" sqref="S28"/>
+      <selection activeCell="U35" sqref="U35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,7 +988,7 @@
         <v>58</v>
       </c>
       <c r="S9">
-        <f>HEX2DEC(RIGHT(R9,LEN(R9)-2))</f>
+        <f t="shared" ref="S9:S40" si="0">HEX2DEC(RIGHT(R9,LEN(R9)-2))</f>
         <v>0</v>
       </c>
       <c r="T9" t="s">
@@ -1030,7 +1030,7 @@
         <v>60</v>
       </c>
       <c r="S10">
-        <f>HEX2DEC(RIGHT(R10,LEN(R10)-2))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="T10" t="s">
@@ -1072,7 +1072,7 @@
         <v>61</v>
       </c>
       <c r="S11">
-        <f>HEX2DEC(RIGHT(R11,LEN(R11)-2))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="T11" t="s">
@@ -1114,7 +1114,7 @@
         <v>62</v>
       </c>
       <c r="S12">
-        <f>HEX2DEC(RIGHT(R12,LEN(R12)-2))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="T12" s="1" t="s">
@@ -1156,7 +1156,7 @@
         <v>63</v>
       </c>
       <c r="S13">
-        <f>HEX2DEC(RIGHT(R13,LEN(R13)-2))</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="T13" t="s">
@@ -1198,7 +1198,7 @@
         <v>64</v>
       </c>
       <c r="S14">
-        <f>HEX2DEC(RIGHT(R14,LEN(R14)-2))</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="T14" t="s">
@@ -1240,7 +1240,7 @@
         <v>65</v>
       </c>
       <c r="S15">
-        <f>HEX2DEC(RIGHT(R15,LEN(R15)-2))</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="T15" t="s">
@@ -1282,7 +1282,7 @@
         <v>66</v>
       </c>
       <c r="S16">
-        <f>HEX2DEC(RIGHT(R16,LEN(R16)-2))</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="T16" t="s">
@@ -1324,7 +1324,7 @@
         <v>67</v>
       </c>
       <c r="S17">
-        <f>HEX2DEC(RIGHT(R17,LEN(R17)-2))</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="V17" t="s">
@@ -1363,7 +1363,7 @@
         <v>68</v>
       </c>
       <c r="S18">
-        <f>HEX2DEC(RIGHT(R18,LEN(R18)-2))</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -1399,7 +1399,7 @@
         <v>69</v>
       </c>
       <c r="S19">
-        <f>HEX2DEC(RIGHT(R19,LEN(R19)-2))</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -1435,7 +1435,7 @@
         <v>70</v>
       </c>
       <c r="S20">
-        <f>HEX2DEC(RIGHT(R20,LEN(R20)-2))</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
@@ -1471,7 +1471,7 @@
         <v>71</v>
       </c>
       <c r="S21">
-        <f>HEX2DEC(RIGHT(R21,LEN(R21)-2))</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
         <v>72</v>
       </c>
       <c r="S22">
-        <f>HEX2DEC(RIGHT(R22,LEN(R22)-2))</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
@@ -1543,7 +1543,7 @@
         <v>73</v>
       </c>
       <c r="S23">
-        <f>HEX2DEC(RIGHT(R23,LEN(R23)-2))</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
@@ -1579,7 +1579,7 @@
         <v>59</v>
       </c>
       <c r="S24">
-        <f>HEX2DEC(RIGHT(R24,LEN(R24)-2))</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -1639,7 +1639,7 @@
         <v>74</v>
       </c>
       <c r="S25">
-        <f>HEX2DEC(RIGHT(R25,LEN(R25)-2))</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="T25" s="1" t="s">
@@ -1708,7 +1708,7 @@
         <v>75</v>
       </c>
       <c r="S26">
-        <f>HEX2DEC(RIGHT(R26,LEN(R26)-2))</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="T26" s="1" t="s">
@@ -1774,7 +1774,7 @@
         <v>76</v>
       </c>
       <c r="S27">
-        <f>HEX2DEC(RIGHT(R27,LEN(R27)-2))</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="T27" t="s">
@@ -1840,7 +1840,7 @@
         <v>77</v>
       </c>
       <c r="S28">
-        <f>HEX2DEC(RIGHT(R28,LEN(R28)-2))</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="T28" t="s">
@@ -1906,7 +1906,7 @@
         <v>78</v>
       </c>
       <c r="S29">
-        <f>HEX2DEC(RIGHT(R29,LEN(R29)-2))</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="T29" t="s">
@@ -1972,7 +1972,7 @@
         <v>79</v>
       </c>
       <c r="S30">
-        <f>HEX2DEC(RIGHT(R30,LEN(R30)-2))</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
@@ -2032,7 +2032,7 @@
         <v>80</v>
       </c>
       <c r="S31">
-        <f>HEX2DEC(RIGHT(R31,LEN(R31)-2))</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
@@ -2068,7 +2068,7 @@
         <v>81</v>
       </c>
       <c r="S32">
-        <f>HEX2DEC(RIGHT(R32,LEN(R32)-2))</f>
+        <f t="shared" si="0"/>
         <v>224</v>
       </c>
       <c r="T32" t="s">
@@ -2110,7 +2110,7 @@
         <v>82</v>
       </c>
       <c r="S33">
-        <f>HEX2DEC(RIGHT(R33,LEN(R33)-2))</f>
+        <f t="shared" si="0"/>
         <v>225</v>
       </c>
       <c r="T33" t="s">
@@ -2152,7 +2152,7 @@
         <v>83</v>
       </c>
       <c r="S34">
-        <f>HEX2DEC(RIGHT(R34,LEN(R34)-2))</f>
+        <f t="shared" si="0"/>
         <v>226</v>
       </c>
       <c r="T34" t="s">
@@ -2194,12 +2194,15 @@
         <v>84</v>
       </c>
       <c r="S35">
-        <f>HEX2DEC(RIGHT(R35,LEN(R35)-2))</f>
+        <f t="shared" si="0"/>
         <v>227</v>
       </c>
       <c r="T35" t="s">
         <v>145</v>
       </c>
+      <c r="U35" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
@@ -2233,7 +2236,7 @@
         <v>85</v>
       </c>
       <c r="S36">
-        <f>HEX2DEC(RIGHT(R36,LEN(R36)-2))</f>
+        <f t="shared" si="0"/>
         <v>228</v>
       </c>
     </row>
@@ -2269,7 +2272,7 @@
         <v>86</v>
       </c>
       <c r="S37">
-        <f>HEX2DEC(RIGHT(R37,LEN(R37)-2))</f>
+        <f t="shared" si="0"/>
         <v>229</v>
       </c>
     </row>
@@ -2305,7 +2308,7 @@
         <v>87</v>
       </c>
       <c r="S38">
-        <f>HEX2DEC(RIGHT(R38,LEN(R38)-2))</f>
+        <f t="shared" si="0"/>
         <v>230</v>
       </c>
     </row>
@@ -2341,7 +2344,7 @@
         <v>88</v>
       </c>
       <c r="S39">
-        <f>HEX2DEC(RIGHT(R39,LEN(R39)-2))</f>
+        <f t="shared" si="0"/>
         <v>231</v>
       </c>
     </row>
@@ -2377,7 +2380,7 @@
         <v>89</v>
       </c>
       <c r="S40">
-        <f>HEX2DEC(RIGHT(R40,LEN(R40)-2))</f>
+        <f t="shared" si="0"/>
         <v>232</v>
       </c>
     </row>
@@ -2413,7 +2416,7 @@
         <v>90</v>
       </c>
       <c r="S41">
-        <f>HEX2DEC(RIGHT(R41,LEN(R41)-2))</f>
+        <f t="shared" ref="S41:S72" si="1">HEX2DEC(RIGHT(R41,LEN(R41)-2))</f>
         <v>233</v>
       </c>
     </row>
@@ -2449,7 +2452,7 @@
         <v>91</v>
       </c>
       <c r="S42">
-        <f>HEX2DEC(RIGHT(R42,LEN(R42)-2))</f>
+        <f t="shared" si="1"/>
         <v>234</v>
       </c>
     </row>
@@ -2485,7 +2488,7 @@
         <v>92</v>
       </c>
       <c r="S43">
-        <f>HEX2DEC(RIGHT(R43,LEN(R43)-2))</f>
+        <f t="shared" si="1"/>
         <v>235</v>
       </c>
     </row>
@@ -2521,7 +2524,7 @@
         <v>93</v>
       </c>
       <c r="S44">
-        <f>HEX2DEC(RIGHT(R44,LEN(R44)-2))</f>
+        <f t="shared" si="1"/>
         <v>236</v>
       </c>
     </row>
@@ -2557,7 +2560,7 @@
         <v>94</v>
       </c>
       <c r="S45">
-        <f>HEX2DEC(RIGHT(R45,LEN(R45)-2))</f>
+        <f t="shared" si="1"/>
         <v>237</v>
       </c>
     </row>
@@ -2593,7 +2596,7 @@
         <v>96</v>
       </c>
       <c r="S46">
-        <f>HEX2DEC(RIGHT(R46,LEN(R46)-2))</f>
+        <f t="shared" si="1"/>
         <v>238</v>
       </c>
     </row>
@@ -2629,7 +2632,7 @@
         <v>95</v>
       </c>
       <c r="S47">
-        <f>HEX2DEC(RIGHT(R47,LEN(R47)-2))</f>
+        <f t="shared" si="1"/>
         <v>239</v>
       </c>
     </row>
@@ -2665,7 +2668,7 @@
         <v>97</v>
       </c>
       <c r="S48">
-        <f>HEX2DEC(RIGHT(R48,LEN(R48)-2))</f>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
     </row>
@@ -2701,7 +2704,7 @@
         <v>98</v>
       </c>
       <c r="S49">
-        <f>HEX2DEC(RIGHT(R49,LEN(R49)-2))</f>
+        <f t="shared" si="1"/>
         <v>241</v>
       </c>
     </row>
@@ -2737,7 +2740,7 @@
         <v>99</v>
       </c>
       <c r="S50">
-        <f>HEX2DEC(RIGHT(R50,LEN(R50)-2))</f>
+        <f t="shared" si="1"/>
         <v>242</v>
       </c>
     </row>
@@ -2773,7 +2776,7 @@
         <v>100</v>
       </c>
       <c r="S51">
-        <f>HEX2DEC(RIGHT(R51,LEN(R51)-2))</f>
+        <f t="shared" si="1"/>
         <v>243</v>
       </c>
     </row>
@@ -2809,7 +2812,7 @@
         <v>101</v>
       </c>
       <c r="S52">
-        <f>HEX2DEC(RIGHT(R52,LEN(R52)-2))</f>
+        <f t="shared" si="1"/>
         <v>244</v>
       </c>
     </row>
@@ -2845,7 +2848,7 @@
         <v>102</v>
       </c>
       <c r="S53">
-        <f>HEX2DEC(RIGHT(R53,LEN(R53)-2))</f>
+        <f t="shared" si="1"/>
         <v>245</v>
       </c>
     </row>
@@ -2881,7 +2884,7 @@
         <v>103</v>
       </c>
       <c r="S54">
-        <f>HEX2DEC(RIGHT(R54,LEN(R54)-2))</f>
+        <f t="shared" si="1"/>
         <v>246</v>
       </c>
     </row>
@@ -2917,7 +2920,7 @@
         <v>104</v>
       </c>
       <c r="S55">
-        <f>HEX2DEC(RIGHT(R55,LEN(R55)-2))</f>
+        <f t="shared" si="1"/>
         <v>247</v>
       </c>
     </row>
@@ -2953,7 +2956,7 @@
         <v>105</v>
       </c>
       <c r="S56">
-        <f>HEX2DEC(RIGHT(R56,LEN(R56)-2))</f>
+        <f t="shared" si="1"/>
         <v>248</v>
       </c>
     </row>
@@ -2989,7 +2992,7 @@
         <v>106</v>
       </c>
       <c r="S57">
-        <f>HEX2DEC(RIGHT(R57,LEN(R57)-2))</f>
+        <f t="shared" si="1"/>
         <v>249</v>
       </c>
     </row>
@@ -3025,7 +3028,7 @@
         <v>107</v>
       </c>
       <c r="S58">
-        <f>HEX2DEC(RIGHT(R58,LEN(R58)-2))</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
     </row>
@@ -3061,7 +3064,7 @@
         <v>108</v>
       </c>
       <c r="S59">
-        <f>HEX2DEC(RIGHT(R59,LEN(R59)-2))</f>
+        <f t="shared" si="1"/>
         <v>251</v>
       </c>
     </row>
@@ -3097,7 +3100,7 @@
         <v>109</v>
       </c>
       <c r="S60">
-        <f>HEX2DEC(RIGHT(R60,LEN(R60)-2))</f>
+        <f t="shared" si="1"/>
         <v>252</v>
       </c>
     </row>
@@ -3133,7 +3136,7 @@
         <v>110</v>
       </c>
       <c r="S61">
-        <f>HEX2DEC(RIGHT(R61,LEN(R61)-2))</f>
+        <f t="shared" si="1"/>
         <v>253</v>
       </c>
     </row>
@@ -3169,7 +3172,7 @@
         <v>111</v>
       </c>
       <c r="S62">
-        <f>HEX2DEC(RIGHT(R62,LEN(R62)-2))</f>
+        <f t="shared" si="1"/>
         <v>254</v>
       </c>
     </row>
@@ -3205,7 +3208,7 @@
         <v>112</v>
       </c>
       <c r="S63">
-        <f>HEX2DEC(RIGHT(R63,LEN(R63)-2))</f>
+        <f t="shared" si="1"/>
         <v>255</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add fixed duration movement; tested orientation/navigation with Shannon
</commit_message>
<xml_diff>
--- a/Host/CommunicationProtocol.xlsx
+++ b/Host/CommunicationProtocol.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="143">
   <si>
     <t>b15</t>
   </si>
@@ -321,51 +321,27 @@
     <t>0xF0</t>
   </si>
   <si>
-    <t>0xF1</t>
-  </si>
-  <si>
     <t>0xF2</t>
   </si>
   <si>
-    <t>0xF3</t>
-  </si>
-  <si>
     <t>0xF4</t>
   </si>
   <si>
-    <t>0xF5</t>
-  </si>
-  <si>
     <t>0xF6</t>
   </si>
   <si>
-    <t>0xF7</t>
-  </si>
-  <si>
     <t>0xF8</t>
   </si>
   <si>
-    <t>0xF9</t>
-  </si>
-  <si>
     <t>0xFA</t>
   </si>
   <si>
-    <t>0xFB</t>
-  </si>
-  <si>
     <t>0xFC</t>
   </si>
   <si>
-    <t>0xFD</t>
-  </si>
-  <si>
     <t>0xFE</t>
   </si>
   <si>
-    <t>0xFF</t>
-  </si>
-  <si>
     <t>For SET commands, assume b08 = 0 (that's how the Arduino handles it)</t>
   </si>
   <si>
@@ -463,6 +439,21 @@
   </si>
   <si>
     <t>Tells all bots to stop moving</t>
+  </si>
+  <si>
+    <t>GO_F</t>
+  </si>
+  <si>
+    <t>goFixed(msb)</t>
+  </si>
+  <si>
+    <t>Tells bot to go for a fixed duration. Data is duration in centiseconds</t>
+  </si>
+  <si>
+    <t>G_GO_F</t>
+  </si>
+  <si>
+    <t>Global version of GO_F</t>
   </si>
 </sst>
 </file>
@@ -789,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X63"/>
+  <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U35" sqref="U35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R48" sqref="R48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,16 +885,16 @@
         <v>57</v>
       </c>
       <c r="S7" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="T7" t="s">
         <v>23</v>
       </c>
       <c r="U7" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="V7" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
@@ -958,7 +949,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
@@ -992,10 +983,10 @@
         <v>0</v>
       </c>
       <c r="T9" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="U9" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
@@ -1037,7 +1028,7 @@
         <v>43</v>
       </c>
       <c r="U10" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
@@ -1079,7 +1070,7 @@
         <v>44</v>
       </c>
       <c r="U11" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
@@ -1118,10 +1109,10 @@
         <v>3</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="U12" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.3">
@@ -1163,7 +1154,7 @@
         <v>45</v>
       </c>
       <c r="U13" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.3">
@@ -1205,7 +1196,7 @@
         <v>46</v>
       </c>
       <c r="U14" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.3">
@@ -1247,12 +1238,12 @@
         <v>47</v>
       </c>
       <c r="U15" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
@@ -1286,10 +1277,10 @@
         <v>7</v>
       </c>
       <c r="T16" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="U16" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.3">
@@ -1328,7 +1319,7 @@
         <v>8</v>
       </c>
       <c r="V17" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
@@ -1646,10 +1637,10 @@
         <v>48</v>
       </c>
       <c r="U25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="V25" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
@@ -1715,7 +1706,7 @@
         <v>49</v>
       </c>
       <c r="U26" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
@@ -1778,10 +1769,10 @@
         <v>22</v>
       </c>
       <c r="T27" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="U27" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
@@ -1847,7 +1838,7 @@
         <v>51</v>
       </c>
       <c r="U28" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
@@ -1913,12 +1904,12 @@
         <v>52</v>
       </c>
       <c r="U29" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>138</v>
       </c>
       <c r="B30" t="s">
         <v>22</v>
@@ -1972,8 +1963,14 @@
         <v>79</v>
       </c>
       <c r="S30">
-        <f t="shared" si="0"/>
+        <f>HEX2DEC(RIGHT(R30,LEN(R30)-2))</f>
         <v>28</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="U30" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
@@ -2075,7 +2072,7 @@
         <v>53</v>
       </c>
       <c r="U32" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
@@ -2117,7 +2114,7 @@
         <v>54</v>
       </c>
       <c r="U33" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -2159,12 +2156,12 @@
         <v>55</v>
       </c>
       <c r="U34" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -2198,10 +2195,10 @@
         <v>227</v>
       </c>
       <c r="T35" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="U35" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
@@ -2416,7 +2413,7 @@
         <v>90</v>
       </c>
       <c r="S41">
-        <f t="shared" ref="S41:S72" si="1">HEX2DEC(RIGHT(R41,LEN(R41)-2))</f>
+        <f t="shared" ref="S41:S63" si="1">HEX2DEC(RIGHT(R41,LEN(R41)-2))</f>
         <v>233</v>
       </c>
     </row>
@@ -2638,7 +2635,7 @@
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>141</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2661,8 +2658,32 @@
       <c r="H48">
         <v>0</v>
       </c>
-      <c r="I48">
-        <v>0</v>
+      <c r="I48" t="s">
+        <v>21</v>
+      </c>
+      <c r="J48" t="s">
+        <v>21</v>
+      </c>
+      <c r="K48" t="s">
+        <v>21</v>
+      </c>
+      <c r="L48" t="s">
+        <v>21</v>
+      </c>
+      <c r="M48" t="s">
+        <v>21</v>
+      </c>
+      <c r="N48" t="s">
+        <v>21</v>
+      </c>
+      <c r="O48" t="s">
+        <v>21</v>
+      </c>
+      <c r="P48" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>21</v>
       </c>
       <c r="R48" t="s">
         <v>97</v>
@@ -2671,6 +2692,12 @@
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
+      <c r="T48" t="s">
+        <v>142</v>
+      </c>
+      <c r="U48" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
@@ -2695,17 +2722,41 @@
         <v>0</v>
       </c>
       <c r="H49">
-        <v>0</v>
-      </c>
-      <c r="I49">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="I49" t="s">
+        <v>21</v>
+      </c>
+      <c r="J49" t="s">
+        <v>21</v>
+      </c>
+      <c r="K49" t="s">
+        <v>21</v>
+      </c>
+      <c r="L49" t="s">
+        <v>21</v>
+      </c>
+      <c r="M49" t="s">
+        <v>21</v>
+      </c>
+      <c r="N49" t="s">
+        <v>21</v>
+      </c>
+      <c r="O49" t="s">
+        <v>21</v>
+      </c>
+      <c r="P49" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>21</v>
       </c>
       <c r="R49" t="s">
         <v>98</v>
       </c>
       <c r="S49">
-        <f t="shared" si="1"/>
-        <v>241</v>
+        <f>HEX2DEC(RIGHT(R49,LEN(R49)-2))</f>
+        <v>242</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.3">
@@ -2728,20 +2779,44 @@
         <v>0</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50">
-        <v>1</v>
-      </c>
-      <c r="I50">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="I50" t="s">
+        <v>21</v>
+      </c>
+      <c r="J50" t="s">
+        <v>21</v>
+      </c>
+      <c r="K50" t="s">
+        <v>21</v>
+      </c>
+      <c r="L50" t="s">
+        <v>21</v>
+      </c>
+      <c r="M50" t="s">
+        <v>21</v>
+      </c>
+      <c r="N50" t="s">
+        <v>21</v>
+      </c>
+      <c r="O50" t="s">
+        <v>21</v>
+      </c>
+      <c r="P50" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>21</v>
       </c>
       <c r="R50" t="s">
         <v>99</v>
       </c>
       <c r="S50">
-        <f t="shared" si="1"/>
-        <v>242</v>
+        <f>HEX2DEC(RIGHT(R50,LEN(R50)-2))</f>
+        <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.3">
@@ -2764,20 +2839,44 @@
         <v>0</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51">
         <v>1</v>
       </c>
-      <c r="I51">
-        <v>1</v>
+      <c r="I51" t="s">
+        <v>21</v>
+      </c>
+      <c r="J51" t="s">
+        <v>21</v>
+      </c>
+      <c r="K51" t="s">
+        <v>21</v>
+      </c>
+      <c r="L51" t="s">
+        <v>21</v>
+      </c>
+      <c r="M51" t="s">
+        <v>21</v>
+      </c>
+      <c r="N51" t="s">
+        <v>21</v>
+      </c>
+      <c r="O51" t="s">
+        <v>21</v>
+      </c>
+      <c r="P51" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>21</v>
       </c>
       <c r="R51" t="s">
         <v>100</v>
       </c>
       <c r="S51">
-        <f t="shared" si="1"/>
-        <v>243</v>
+        <f>HEX2DEC(RIGHT(R51,LEN(R51)-2))</f>
+        <v>246</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.3">
@@ -2797,23 +2896,47 @@
         <v>1</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H52">
         <v>0</v>
       </c>
-      <c r="I52">
-        <v>0</v>
+      <c r="I52" t="s">
+        <v>21</v>
+      </c>
+      <c r="J52" t="s">
+        <v>21</v>
+      </c>
+      <c r="K52" t="s">
+        <v>21</v>
+      </c>
+      <c r="L52" t="s">
+        <v>21</v>
+      </c>
+      <c r="M52" t="s">
+        <v>21</v>
+      </c>
+      <c r="N52" t="s">
+        <v>21</v>
+      </c>
+      <c r="O52" t="s">
+        <v>21</v>
+      </c>
+      <c r="P52" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>21</v>
       </c>
       <c r="R52" t="s">
         <v>101</v>
       </c>
       <c r="S52">
-        <f t="shared" si="1"/>
-        <v>244</v>
+        <f>HEX2DEC(RIGHT(R52,LEN(R52)-2))</f>
+        <v>248</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.3">
@@ -2833,23 +2956,47 @@
         <v>1</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="I53">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="I53" t="s">
+        <v>21</v>
+      </c>
+      <c r="J53" t="s">
+        <v>21</v>
+      </c>
+      <c r="K53" t="s">
+        <v>21</v>
+      </c>
+      <c r="L53" t="s">
+        <v>21</v>
+      </c>
+      <c r="M53" t="s">
+        <v>21</v>
+      </c>
+      <c r="N53" t="s">
+        <v>21</v>
+      </c>
+      <c r="O53" t="s">
+        <v>21</v>
+      </c>
+      <c r="P53" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>21</v>
       </c>
       <c r="R53" t="s">
         <v>102</v>
       </c>
       <c r="S53">
-        <f t="shared" si="1"/>
-        <v>245</v>
+        <f>HEX2DEC(RIGHT(R53,LEN(R53)-2))</f>
+        <v>250</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.3">
@@ -2869,23 +3016,47 @@
         <v>1</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G54">
         <v>1</v>
       </c>
       <c r="H54">
-        <v>1</v>
-      </c>
-      <c r="I54">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="I54" t="s">
+        <v>21</v>
+      </c>
+      <c r="J54" t="s">
+        <v>21</v>
+      </c>
+      <c r="K54" t="s">
+        <v>21</v>
+      </c>
+      <c r="L54" t="s">
+        <v>21</v>
+      </c>
+      <c r="M54" t="s">
+        <v>21</v>
+      </c>
+      <c r="N54" t="s">
+        <v>21</v>
+      </c>
+      <c r="O54" t="s">
+        <v>21</v>
+      </c>
+      <c r="P54" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>21</v>
       </c>
       <c r="R54" t="s">
         <v>103</v>
       </c>
       <c r="S54">
-        <f t="shared" si="1"/>
-        <v>246</v>
+        <f>HEX2DEC(RIGHT(R54,LEN(R54)-2))</f>
+        <v>252</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.3">
@@ -2905,7 +3076,7 @@
         <v>1</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G55">
         <v>1</v>
@@ -2913,303 +3084,39 @@
       <c r="H55">
         <v>1</v>
       </c>
-      <c r="I55">
-        <v>1</v>
+      <c r="I55" t="s">
+        <v>21</v>
+      </c>
+      <c r="J55" t="s">
+        <v>21</v>
+      </c>
+      <c r="K55" t="s">
+        <v>21</v>
+      </c>
+      <c r="L55" t="s">
+        <v>21</v>
+      </c>
+      <c r="M55" t="s">
+        <v>21</v>
+      </c>
+      <c r="N55" t="s">
+        <v>21</v>
+      </c>
+      <c r="O55" t="s">
+        <v>21</v>
+      </c>
+      <c r="P55" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>21</v>
       </c>
       <c r="R55" t="s">
         <v>104</v>
       </c>
       <c r="S55">
-        <f t="shared" si="1"/>
-        <v>247</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>32</v>
-      </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
-      <c r="F56">
-        <v>1</v>
-      </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56">
-        <v>0</v>
-      </c>
-      <c r="R56" t="s">
-        <v>105</v>
-      </c>
-      <c r="S56">
-        <f t="shared" si="1"/>
-        <v>248</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>32</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-      <c r="F57">
-        <v>1</v>
-      </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="I57">
-        <v>1</v>
-      </c>
-      <c r="R57" t="s">
-        <v>106</v>
-      </c>
-      <c r="S57">
-        <f t="shared" si="1"/>
-        <v>249</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>32</v>
-      </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="E58">
-        <v>1</v>
-      </c>
-      <c r="F58">
-        <v>1</v>
-      </c>
-      <c r="G58">
-        <v>0</v>
-      </c>
-      <c r="H58">
-        <v>1</v>
-      </c>
-      <c r="I58">
-        <v>0</v>
-      </c>
-      <c r="R58" t="s">
-        <v>107</v>
-      </c>
-      <c r="S58">
-        <f t="shared" si="1"/>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>32</v>
-      </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59">
-        <v>1</v>
-      </c>
-      <c r="F59">
-        <v>1</v>
-      </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
-        <v>1</v>
-      </c>
-      <c r="I59">
-        <v>1</v>
-      </c>
-      <c r="R59" t="s">
-        <v>108</v>
-      </c>
-      <c r="S59">
-        <f t="shared" si="1"/>
-        <v>251</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>32</v>
-      </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-      <c r="F60">
-        <v>1</v>
-      </c>
-      <c r="G60">
-        <v>1</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="I60">
-        <v>0</v>
-      </c>
-      <c r="R60" t="s">
-        <v>109</v>
-      </c>
-      <c r="S60">
-        <f t="shared" si="1"/>
-        <v>252</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>32</v>
-      </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="E61">
-        <v>1</v>
-      </c>
-      <c r="F61">
-        <v>1</v>
-      </c>
-      <c r="G61">
-        <v>1</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-      <c r="I61">
-        <v>1</v>
-      </c>
-      <c r="R61" t="s">
-        <v>110</v>
-      </c>
-      <c r="S61">
-        <f t="shared" si="1"/>
-        <v>253</v>
-      </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>32</v>
-      </c>
-      <c r="B62">
-        <v>1</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-      <c r="D62">
-        <v>1</v>
-      </c>
-      <c r="E62">
-        <v>1</v>
-      </c>
-      <c r="F62">
-        <v>1</v>
-      </c>
-      <c r="G62">
-        <v>1</v>
-      </c>
-      <c r="H62">
-        <v>1</v>
-      </c>
-      <c r="I62">
-        <v>0</v>
-      </c>
-      <c r="R62" t="s">
-        <v>111</v>
-      </c>
-      <c r="S62">
-        <f t="shared" si="1"/>
+        <f>HEX2DEC(RIGHT(R55,LEN(R55)-2))</f>
         <v>254</v>
-      </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>32</v>
-      </c>
-      <c r="B63">
-        <v>1</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="E63">
-        <v>1</v>
-      </c>
-      <c r="F63">
-        <v>1</v>
-      </c>
-      <c r="G63">
-        <v>1</v>
-      </c>
-      <c r="H63">
-        <v>1</v>
-      </c>
-      <c r="I63">
-        <v>1</v>
-      </c>
-      <c r="R63" t="s">
-        <v>112</v>
-      </c>
-      <c r="S63">
-        <f t="shared" si="1"/>
-        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3351,7 +3258,7 @@
         <v>0</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
@@ -3365,7 +3272,7 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -3383,12 +3290,12 @@
         <v>1</v>
       </c>
       <c r="S4" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -3439,7 +3346,7 @@
         <v>21</v>
       </c>
       <c r="S5" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get dead reckoning implemented
</commit_message>
<xml_diff>
--- a/Host/CommunicationProtocol.xlsx
+++ b/Host/CommunicationProtocol.xlsx
@@ -1,31 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AppleMath\Documents\APSC200_2019\SWEP-2019\Host\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jared/Documents/SWEP/SWEP-2019/Host/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE01A33-D864-AC4F-BABB-ED70A14A8CE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bot-side" sheetId="1" r:id="rId1"/>
     <sheet name="Host-side" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="154">
   <si>
     <t>b15</t>
   </si>
@@ -420,9 +427,6 @@
     <t>dontGo()</t>
   </si>
   <si>
-    <t>All unallocated instruction default to badResponse()</t>
-  </si>
-  <si>
     <t>Indicates bot is good to go</t>
   </si>
   <si>
@@ -472,12 +476,30 @@
   </si>
   <si>
     <t>Gets angle from all bots</t>
+  </si>
+  <si>
+    <t>GET_POS</t>
+  </si>
+  <si>
+    <t>Gets bot's X, Y, theta, and timestamp (Special command)</t>
+  </si>
+  <si>
+    <t>getPos()</t>
+  </si>
+  <si>
+    <t>RESP_POS</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>This response has bot ID in most significant byte, followed by the raw 32 bit float values for X, Y, theta, and 32 bit unsigned long. Total is 17 bytes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -797,25 +819,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+    <sheetView zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="17" width="4" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6" customWidth="1"/>
-    <col min="19" max="19" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="43.109375" customWidth="1"/>
+    <col min="19" max="19" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="43.1640625" customWidth="1"/>
     <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="22" width="34.77734375" customWidth="1"/>
+    <col min="22" max="22" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="S1" s="2" t="s">
         <v>38</v>
       </c>
@@ -825,7 +847,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="S2" s="2" t="s">
         <v>39</v>
       </c>
@@ -835,7 +857,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="S3" s="3" t="s">
         <v>40</v>
       </c>
@@ -845,7 +867,7 @@
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="S4" s="3" t="s">
         <v>56</v>
       </c>
@@ -855,7 +877,7 @@
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
     </row>
-    <row r="5" spans="1:24" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="S5" s="3" t="s">
         <v>41</v>
       </c>
@@ -865,7 +887,7 @@
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
     </row>
-    <row r="6" spans="1:24" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="S6" s="3" t="s">
         <v>42</v>
       </c>
@@ -875,7 +897,7 @@
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -903,7 +925,7 @@
         <v>57</v>
       </c>
       <c r="S7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T7" t="s">
         <v>23</v>
@@ -915,7 +937,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -965,7 +987,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -1007,7 +1029,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1049,7 +1071,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1091,7 +1113,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1133,7 +1155,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1175,7 +1197,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1217,7 +1239,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1259,7 +1281,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>125</v>
       </c>
@@ -1301,9 +1323,9 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>148</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
@@ -1336,11 +1358,14 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="V17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="T17" t="s">
+        <v>149</v>
+      </c>
+      <c r="U17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1376,7 +1401,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1412,7 +1437,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1448,7 +1473,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1484,7 +1509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1520,7 +1545,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1556,7 +1581,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1592,7 +1617,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1661,7 +1686,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1727,7 +1752,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1793,7 +1818,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1859,7 +1884,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1925,9 +1950,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B30" t="s">
         <v>22</v>
@@ -1985,13 +2010,13 @@
         <v>28</v>
       </c>
       <c r="T30" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U30" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -2051,7 +2076,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -2093,7 +2118,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -2135,7 +2160,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -2177,9 +2202,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -2213,15 +2238,15 @@
         <v>227</v>
       </c>
       <c r="T35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="U35" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -2255,15 +2280,15 @@
         <v>228</v>
       </c>
       <c r="T36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="U36" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -2297,15 +2322,15 @@
         <v>229</v>
       </c>
       <c r="T37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="U37" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -2339,13 +2364,13 @@
         <v>230</v>
       </c>
       <c r="T38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="U38" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -2381,7 +2406,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -2417,7 +2442,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -2453,7 +2478,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>32</v>
       </c>
@@ -2489,7 +2514,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>32</v>
       </c>
@@ -2525,7 +2550,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>32</v>
       </c>
@@ -2561,7 +2586,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>32</v>
       </c>
@@ -2597,7 +2622,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>32</v>
       </c>
@@ -2633,7 +2658,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>32</v>
       </c>
@@ -2669,9 +2694,9 @@
         <v>239</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2729,13 +2754,13 @@
         <v>240</v>
       </c>
       <c r="T48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="U48" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -2795,7 +2820,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>32</v>
       </c>
@@ -2855,7 +2880,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>32</v>
       </c>
@@ -2915,7 +2940,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -2975,7 +3000,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>32</v>
       </c>
@@ -3035,7 +3060,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>32</v>
       </c>
@@ -3095,7 +3120,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>32</v>
       </c>
@@ -3172,22 +3197,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="17" width="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.5546875" customWidth="1"/>
+    <col min="19" max="19" width="40.5" customWidth="1"/>
     <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -3215,7 +3240,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -3265,7 +3290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3294,10 +3319,10 @@
         <v>0</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -3326,10 +3351,10 @@
         <v>1</v>
       </c>
       <c r="S4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -3382,7 +3407,42 @@
         <v>21</v>
       </c>
       <c r="S5" t="s">
-        <v>133</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
+        <v>152</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement XBee class hierarchy in MATLAB for host; redesign communication spec for use in XBee API mode
</commit_message>
<xml_diff>
--- a/Host/CommunicationProtocol.xlsx
+++ b/Host/CommunicationProtocol.xlsx
@@ -1,24 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AppleMath\Documents\APSC200_2019\SWEP-2019\Host\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jared/Documents/SWEP/SWEP-2019/Host/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9F1BB1-0A6A-564D-9B30-F1D725FDCBAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bot-side" sheetId="1" r:id="rId1"/>
     <sheet name="Host-side" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -477,7 +484,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -797,25 +804,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="17" width="4" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6" customWidth="1"/>
-    <col min="19" max="19" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="43.109375" customWidth="1"/>
+    <col min="19" max="19" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="43.1640625" customWidth="1"/>
     <col min="21" max="21" width="14.33203125" customWidth="1"/>
-    <col min="22" max="22" width="34.77734375" customWidth="1"/>
+    <col min="22" max="22" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="S1" s="2" t="s">
         <v>38</v>
       </c>
@@ -825,7 +832,7 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="S2" s="2" t="s">
         <v>39</v>
       </c>
@@ -835,7 +842,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="S3" s="3" t="s">
         <v>40</v>
       </c>
@@ -845,7 +852,7 @@
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="S4" s="3" t="s">
         <v>56</v>
       </c>
@@ -855,7 +862,7 @@
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
     </row>
-    <row r="5" spans="1:24" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="S5" s="3" t="s">
         <v>41</v>
       </c>
@@ -865,7 +872,7 @@
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
     </row>
-    <row r="6" spans="1:24" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="S6" s="3" t="s">
         <v>42</v>
       </c>
@@ -875,7 +882,7 @@
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -915,7 +922,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -965,7 +972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -1007,7 +1014,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1049,7 +1056,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1091,7 +1098,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1133,7 +1140,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1175,7 +1182,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1217,7 +1224,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1259,7 +1266,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>125</v>
       </c>
@@ -1301,7 +1308,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1340,7 +1347,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1376,7 +1383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1412,7 +1419,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1448,7 +1455,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1484,7 +1491,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1520,7 +1527,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1556,7 +1563,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1592,7 +1599,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1661,7 +1668,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1727,7 +1734,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1793,7 +1800,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1859,7 +1866,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1925,7 +1932,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>138</v>
       </c>
@@ -1991,7 +1998,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -2051,7 +2058,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -2093,7 +2100,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -2135,7 +2142,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -2177,7 +2184,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>136</v>
       </c>
@@ -2219,7 +2226,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -2261,7 +2268,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -2303,7 +2310,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>145</v>
       </c>
@@ -2345,7 +2352,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -2381,7 +2388,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -2417,7 +2424,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -2453,7 +2460,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>32</v>
       </c>
@@ -2489,7 +2496,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>32</v>
       </c>
@@ -2525,7 +2532,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>32</v>
       </c>
@@ -2561,7 +2568,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>32</v>
       </c>
@@ -2597,7 +2604,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>32</v>
       </c>
@@ -2633,7 +2640,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>32</v>
       </c>
@@ -2669,7 +2676,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>141</v>
       </c>
@@ -2735,7 +2742,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -2795,7 +2802,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>32</v>
       </c>
@@ -2855,7 +2862,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>32</v>
       </c>
@@ -2915,7 +2922,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -2975,7 +2982,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>32</v>
       </c>
@@ -3035,7 +3042,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>32</v>
       </c>
@@ -3095,7 +3102,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>32</v>
       </c>
@@ -3172,22 +3179,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="17" width="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.5546875" customWidth="1"/>
+    <col min="19" max="19" width="40.5" customWidth="1"/>
     <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -3215,7 +3222,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -3265,7 +3272,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3297,7 +3304,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -3329,7 +3336,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>129</v>
       </c>

</xml_diff>